<commit_message>
add more test & cleanup
</commit_message>
<xml_diff>
--- a/backend/hct_mis_api/apps/payment/tests/test_file/import_file_reference_id.xlsx
+++ b/backend/hct_mis_api/apps/payment/tests/test_file/import_file_reference_id.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
   <si>
     <t>payment_id</t>
   </si>
@@ -49,16 +49,25 @@
     <t>reference_id</t>
   </si>
   <si>
+    <t>transaction_status_blockchain</t>
+  </si>
+  <si>
     <t>RCPT-0060-24-0.000.665</t>
   </si>
   <si>
     <t>ref1</t>
   </si>
   <si>
+    <t>transaction_status_blockchain_link</t>
+  </si>
+  <si>
     <t>RCPT-0060-24-0.000.666</t>
   </si>
   <si>
     <t>ref2</t>
+  </si>
+  <si>
+    <t>www_link</t>
   </si>
 </sst>
 </file>
@@ -577,7 +586,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -607,7 +615,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -633,7 +640,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -659,7 +665,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -685,7 +690,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -711,7 +715,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -737,7 +740,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -763,7 +765,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -789,7 +790,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -815,7 +815,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -872,7 +871,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -898,7 +896,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -924,7 +921,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -950,7 +946,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -976,7 +971,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1002,7 +996,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1028,7 +1021,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1054,7 +1046,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1080,7 +1071,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1106,7 +1096,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1154,7 +1143,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1184,7 +1172,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1210,7 +1197,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1236,7 +1222,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1262,7 +1247,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1288,7 +1272,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1314,7 +1297,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1340,7 +1322,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1366,7 +1347,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1392,7 +1372,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1418,14 +1397,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="12" width="20" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.85156" style="1" customWidth="1"/>
+    <col min="13" max="13" width="42.3906" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
@@ -1465,10 +1445,13 @@
       <c r="L1" t="s" s="2">
         <v>11</v>
       </c>
+      <c r="M1" t="s" s="2">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1489,12 +1472,15 @@
         <v>45051</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="M2" t="s" s="2">
+        <v>15</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -1515,7 +1501,10 @@
         <v>45051</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="M3" t="s" s="2">
+        <v>18</v>
       </c>
     </row>
     <row r="4" ht="13.55" customHeight="1">
@@ -1531,6 +1520,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="8"/>
       <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
       <c r="A5" s="10"/>
@@ -1545,6 +1535,7 @@
       <c r="J5" s="11"/>
       <c r="K5" s="12"/>
       <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
       <c r="A6" s="10"/>
@@ -1559,6 +1550,7 @@
       <c r="J6" s="11"/>
       <c r="K6" s="12"/>
       <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
       <c r="A7" s="10"/>
@@ -1573,6 +1565,7 @@
       <c r="J7" s="11"/>
       <c r="K7" s="12"/>
       <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
       <c r="A8" s="10"/>
@@ -1587,6 +1580,7 @@
       <c r="J8" s="11"/>
       <c r="K8" s="12"/>
       <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
       <c r="A9" s="10"/>
@@ -1601,6 +1595,7 @@
       <c r="J9" s="11"/>
       <c r="K9" s="12"/>
       <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
       <c r="A10" s="14"/>
@@ -1615,6 +1610,7 @@
       <c r="J10" s="15"/>
       <c r="K10" s="16"/>
       <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>